<commit_message>
update example with the last version of epanet.m
</commit_message>
<xml_diff>
--- a/networks/exeter-benchmarks/D-Town Water Distribution Network BWN-II/Original_BWNII/10_Guidolin.xlsx
+++ b/networks/exeter-benchmarks/D-Town Water Distribution Network BWN-II/Original_BWNII/10_Guidolin.xlsx
@@ -3295,201 +3295,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C36E55CDBA0CA346ABBE29398E6C1443" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="97dc9f8f7e8fc0ddc41aea005ff7fc5e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfcc3db1-e1e4-4837-9810-7b1d4351df11" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bffe94494bc0c34d7a0d5c1f4ad07516" ns2:_="">
-    <xsd:import namespace="cfcc3db1-e1e4-4837-9810-7b1d4351df11"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cfcc3db1-e1e4-4837-9810-7b1d4351df11" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="11" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="fc5b67b3-f07b-4a01-9212-9530f3790bcd" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfcc3db1-e1e4-4837-9810-7b1d4351df11">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB42631C-162D-4E95-B55A-0F36CF7CE874}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95106C3A-012E-45F2-9E76-C4BF2168DE36}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C34B189-07F4-4199-B739-5AF952F5ADE8}"/>
 </file>
</xml_diff>